<commit_message>
Update for calibration, usinf multiple reference weights. Preparation of using 2 sensors together.
</commit_message>
<xml_diff>
--- a/src/ratio_calc.xlsx
+++ b/src/ratio_calc.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17668"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hristo\raspberryPi\raspberrypipythonelectronicscaletime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hristo\projects\pocs\python\ya_hx711py\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1 Sensor" sheetId="1" r:id="rId1"/>
+    <sheet name="2 Sensors" sheetId="2" r:id="rId2"/>
+    <sheet name="1Sensor Orig" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,21 +26,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>Ref weights:</t>
   </si>
   <si>
-    <t>0ffset:</t>
-  </si>
-  <si>
     <t>Ratios:</t>
   </si>
   <si>
     <t>r = (w - o)/ref w</t>
   </si>
   <si>
-    <t>Offset:</t>
+    <t>2 Sensors combined</t>
+  </si>
+  <si>
+    <t>0ffset (Sensor 1 + Sensor 2):</t>
+  </si>
+  <si>
+    <t>Offset (S1+S2)</t>
+  </si>
+  <si>
+    <t>Offsets (S1+S2)</t>
+  </si>
+  <si>
+    <t>1 Sensor</t>
+  </si>
+  <si>
+    <t>0ffset (Sensor):</t>
+  </si>
+  <si>
+    <t>Offset (Sensor):</t>
+  </si>
+  <si>
+    <t>Offsets:</t>
+  </si>
+  <si>
+    <t>Average ratio</t>
+  </si>
+  <si>
+    <t>Average ratio:</t>
+  </si>
+  <si>
+    <t>Average ratios:</t>
   </si>
 </sst>
 </file>
@@ -48,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +85,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,15 +114,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,186 +453,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>25</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>75</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>150</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>225</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>300</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>375</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>475</v>
       </c>
-      <c r="H2">
-        <v>550</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8670386.5332999993</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8752399.9066700004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8876659.7200000007</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9001015.1866699997</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9125726.5800000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9249752.4866700005</v>
+      </c>
+      <c r="H4" s="1">
+        <v>9415005.6466700006</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8628270.3399999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>8670386.5332999993</v>
-      </c>
-      <c r="B3" s="1">
-        <v>8752399.9066700004</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8876659.7200000007</v>
-      </c>
-      <c r="D3" s="1">
-        <v>9001015.1866699997</v>
-      </c>
-      <c r="E3" s="1">
-        <v>9125726.5800000001</v>
-      </c>
-      <c r="F3" s="1">
-        <v>9249752.4866700005</v>
-      </c>
-      <c r="G3" s="1">
-        <v>9415005.6466700006</v>
-      </c>
-      <c r="K3" s="1">
-        <v>8628270.3399999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7">
+        <f>(B4-J4)/B3</f>
+        <v>1684.6477319999785</v>
+      </c>
+      <c r="C7">
+        <f>(C4-J4)/C3</f>
+        <v>1655.0608889333407</v>
+      </c>
+      <c r="D7">
+        <f>(D4-J4)/D3</f>
+        <v>1655.9292000000055</v>
+      </c>
+      <c r="E7">
+        <f>(E4-J4)/E3</f>
+        <v>1656.6437629777772</v>
+      </c>
+      <c r="F7">
+        <f>(F4-J4)/F3</f>
+        <v>1658.1874666666674</v>
+      </c>
+      <c r="G7">
+        <f>(G4-J4)/G3</f>
+        <v>1657.285724453335</v>
+      </c>
+      <c r="H7">
+        <f>(H4-J4)/H3</f>
+        <v>1656.28485614737</v>
+      </c>
+      <c r="J7">
+        <f>SUM(B7:H7)/7</f>
+        <v>1660.5770901683536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>(A3-K3)/A2</f>
-        <v>1684.6477319999785</v>
-      </c>
-      <c r="B6">
-        <f>(B3-K3)/B2</f>
-        <v>1655.0608889333407</v>
-      </c>
-      <c r="C6">
-        <f>(C3-K3)/C2</f>
-        <v>1655.9292000000055</v>
-      </c>
-      <c r="D6">
-        <f>(D3-K3)/D2</f>
-        <v>1656.6437629777772</v>
-      </c>
-      <c r="E6">
-        <f>(E3-K3)/E2</f>
-        <v>1658.1874666666674</v>
-      </c>
-      <c r="F6">
-        <f>(F3-K3)/F2</f>
-        <v>1657.285724453335</v>
-      </c>
-      <c r="G6">
-        <f>(G3-K3)/G2</f>
-        <v>1656.28485614737</v>
-      </c>
-      <c r="H6">
-        <f>(H3-K3)/H2</f>
-        <v>-15687.764254545455</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="C14">
         <v>100</v>
       </c>
-      <c r="C13">
+      <c r="D14">
         <v>175</v>
       </c>
-      <c r="D13">
+      <c r="E14">
         <v>250</v>
       </c>
-      <c r="K13" s="1">
+      <c r="J14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8671186.0600000005</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8794613.3066700008</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8918932.9733300004</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9043501.5133299995</v>
+      </c>
+      <c r="J15" s="1">
         <v>8628906.7799999993</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>8671186.0600000005</v>
-      </c>
-      <c r="B14" s="1">
-        <v>8794613.3066700008</v>
-      </c>
-      <c r="C14" s="1">
-        <v>8918932.9733300004</v>
-      </c>
-      <c r="D14" s="1">
-        <v>9043501.5133299995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>(A14-K13)/A13</f>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>(B15-J15)/B14</f>
         <v>1691.1712000000477</v>
       </c>
-      <c r="B17">
-        <f>(B14-K13)/B13</f>
+      <c r="C18">
+        <f>(C15-J15)/C14</f>
         <v>1657.0652667000145</v>
       </c>
-      <c r="C17">
-        <f>(C14-K13)/C13</f>
+      <c r="D18">
+        <f>(D15-J15)/D14</f>
         <v>1657.2925333142919</v>
       </c>
-      <c r="D17">
-        <f>(D14-K13)/D13</f>
+      <c r="E18">
+        <f>(E15-J15)/E14</f>
         <v>1658.3789333200007</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="J18">
+        <f>SUM(B18:E18)/4</f>
+        <v>1665.9769833335886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>8670637.7733299993</v>
       </c>
     </row>
@@ -581,4 +662,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3">
+        <v>225</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3">
+        <v>375</v>
+      </c>
+      <c r="H3">
+        <v>475</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f>(B4-J4)/B3</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>(C4-J4)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>(D4-J4)/D3</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>(E4-J4)/E3</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>(F4-J4)/F3</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>(G4-J4)/G3</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>(H4-J4)/H3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>175</v>
+      </c>
+      <c r="E14">
+        <v>250</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>(B15-J14)/B14</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>(C15-J14)/C14</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>(D15-J14)/D14</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>(E15-J14)/E14</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3">
+        <v>225</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3">
+        <v>375</v>
+      </c>
+      <c r="H3">
+        <v>475</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8670386.5332999993</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8752399.9066700004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8876659.7200000007</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9001015.1866699997</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9125726.5800000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9249752.4866700005</v>
+      </c>
+      <c r="H4" s="1">
+        <v>9415005.6466700006</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8628270.3399999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f>(B4-J4)/B3</f>
+        <v>1684.6477319999785</v>
+      </c>
+      <c r="C7">
+        <f>(C4-J4)/C3</f>
+        <v>1655.0608889333407</v>
+      </c>
+      <c r="D7">
+        <f>(D4-J4)/D3</f>
+        <v>1655.9292000000055</v>
+      </c>
+      <c r="E7">
+        <f>(E4-J4)/E3</f>
+        <v>1656.6437629777772</v>
+      </c>
+      <c r="F7">
+        <f>(F4-J4)/F3</f>
+        <v>1658.1874666666674</v>
+      </c>
+      <c r="G7">
+        <f>(G4-J4)/G3</f>
+        <v>1657.285724453335</v>
+      </c>
+      <c r="H7">
+        <f>(H4-J4)/H3</f>
+        <v>1656.28485614737</v>
+      </c>
+      <c r="J7">
+        <f>SUM(C7:H7)/6</f>
+        <v>1656.565316529749</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>175</v>
+      </c>
+      <c r="E14">
+        <v>250</v>
+      </c>
+      <c r="J14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8671186.0600000005</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8794613.3066700008</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8918932.9733300004</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9043501.5133299995</v>
+      </c>
+      <c r="J15" s="1">
+        <v>8628906.7799999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>(B15-J15)/B14</f>
+        <v>1691.1712000000477</v>
+      </c>
+      <c r="C18">
+        <f>(C15-J15)/C14</f>
+        <v>1657.0652667000145</v>
+      </c>
+      <c r="D18">
+        <f>(D15-J15)/D14</f>
+        <v>1657.2925333142919</v>
+      </c>
+      <c r="E18">
+        <f>(E15-J15)/E14</f>
+        <v>1658.3789333200007</v>
+      </c>
+      <c r="J18">
+        <f>SUM(B18:E18)/4</f>
+        <v>1665.9769833335886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8670637.7733299993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial support of 2 HX711 working together... not tested yet.
</commit_message>
<xml_diff>
--- a/src/ratio_calc.xlsx
+++ b/src/ratio_calc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="1 Sensor" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
   <si>
     <t>Ref weights:</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Average ratios:</t>
+  </si>
+  <si>
+    <t>Sensor 1</t>
+  </si>
+  <si>
+    <t>Sensor 2</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,8 +481,17 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -653,9 +668,193 @@
         <v>1665.9769833335886</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8670637.7733299993</v>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>150</v>
+      </c>
+      <c r="E23">
+        <v>225</v>
+      </c>
+      <c r="F23">
+        <v>300</v>
+      </c>
+      <c r="G23">
+        <v>375</v>
+      </c>
+      <c r="H23">
+        <v>475</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8670386.5332999993</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8752399.9066700004</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8876659.7200000007</v>
+      </c>
+      <c r="E24" s="1">
+        <v>9001015.1866699997</v>
+      </c>
+      <c r="F24" s="1">
+        <v>9125726.5800000001</v>
+      </c>
+      <c r="G24" s="1">
+        <v>9249752.4866700005</v>
+      </c>
+      <c r="H24" s="1">
+        <v>9415005.6466700006</v>
+      </c>
+      <c r="J24" s="1">
+        <v>8628270.3399999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <f>(B24-J24)/B23</f>
+        <v>1684.6477319999785</v>
+      </c>
+      <c r="C27">
+        <f>(C24-J24)/C23</f>
+        <v>1655.0608889333407</v>
+      </c>
+      <c r="D27">
+        <f>(D24-J24)/D23</f>
+        <v>1655.9292000000055</v>
+      </c>
+      <c r="E27">
+        <f>(E24-J24)/E23</f>
+        <v>1656.6437629777772</v>
+      </c>
+      <c r="F27">
+        <f>(F24-J24)/F23</f>
+        <v>1658.1874666666674</v>
+      </c>
+      <c r="G27">
+        <f>(G24-J24)/G23</f>
+        <v>1657.285724453335</v>
+      </c>
+      <c r="H27">
+        <f>(H24-J24)/H23</f>
+        <v>1656.28485614737</v>
+      </c>
+      <c r="J27">
+        <f>SUM(B27:H27)/7</f>
+        <v>1660.5770901683536</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>175</v>
+      </c>
+      <c r="E34">
+        <v>250</v>
+      </c>
+      <c r="J34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="1">
+        <v>8671186.0600000005</v>
+      </c>
+      <c r="C35" s="1">
+        <v>8794613.3066700008</v>
+      </c>
+      <c r="D35" s="1">
+        <v>8918932.9733300004</v>
+      </c>
+      <c r="E35" s="1">
+        <v>9043501.5133299995</v>
+      </c>
+      <c r="J35" s="1">
+        <v>8628906.7799999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <f>(B35-J35)/B34</f>
+        <v>1691.1712000000477</v>
+      </c>
+      <c r="C38">
+        <f>(C35-J35)/C34</f>
+        <v>1657.0652667000145</v>
+      </c>
+      <c r="D38">
+        <f>(D35-J35)/D34</f>
+        <v>1657.2925333142919</v>
+      </c>
+      <c r="E38">
+        <f>(E35-J35)/E34</f>
+        <v>1658.3789333200007</v>
+      </c>
+      <c r="J38">
+        <f>SUM(B38:E38)/4</f>
+        <v>1665.9769833335886</v>
       </c>
     </row>
   </sheetData>
@@ -668,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some calibration data. WiP...
</commit_message>
<xml_diff>
--- a/src/ratio_calc.xlsx
+++ b/src/ratio_calc.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17668"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hristo\projects\pocs\python\ya_hx711py\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hristo\git\ya_hx711py\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9F67F59D-9C33-4CC1-9182-28F08D562B11}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1 Sensor" sheetId="1" r:id="rId1"/>
-    <sheet name="2 Sensors" sheetId="2" r:id="rId2"/>
-    <sheet name="1Sensor Orig" sheetId="3" r:id="rId3"/>
+    <sheet name="2 Sensors (2)" sheetId="4" r:id="rId1"/>
+    <sheet name="1 Sensor" sheetId="1" r:id="rId2"/>
+    <sheet name="2 Sensors" sheetId="2" r:id="rId3"/>
+    <sheet name="1Sensor Orig" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>Ref weights:</t>
   </si>
@@ -74,12 +76,15 @@
   </si>
   <si>
     <t>Sensor 2</t>
+  </si>
+  <si>
+    <t>Offset w/o anything</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -458,11 +463,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA82A29-B9AD-488E-86C1-B679C36AA7D7}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3">
+        <v>225</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3">
+        <v>375</v>
+      </c>
+      <c r="H3">
+        <v>475</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>18268919.776000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>18304986.135000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>18356977.618999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>18422516.526000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>18449322.964000002</v>
+      </c>
+      <c r="G4" s="1">
+        <v>18514402.952</v>
+      </c>
+      <c r="H4" s="1">
+        <v>18560397.458999999</v>
+      </c>
+      <c r="J4" s="1">
+        <v>18229794.022999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f>(B4-J4)/B3</f>
+        <v>1565.0301200000943</v>
+      </c>
+      <c r="C7">
+        <f>(C4-J4)/C3</f>
+        <v>1002.5614933333794</v>
+      </c>
+      <c r="D7">
+        <f>(D4-J4)/D3</f>
+        <v>847.89064000000553</v>
+      </c>
+      <c r="E7">
+        <f>(E4-J4)/E3</f>
+        <v>856.54445777778824</v>
+      </c>
+      <c r="F7">
+        <f>(F4-J4)/F3</f>
+        <v>731.76313666667784</v>
+      </c>
+      <c r="G7">
+        <f>(G4-J4)/G3</f>
+        <v>758.95714400000372</v>
+      </c>
+      <c r="H7">
+        <f>(H4-J4)/H3</f>
+        <v>696.007233684212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>175</v>
+      </c>
+      <c r="E14">
+        <v>250</v>
+      </c>
+      <c r="J14" s="1">
+        <v>18229794.022999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18268919.776000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>18320473.491</v>
+      </c>
+      <c r="D15" s="1">
+        <v>18375631.173</v>
+      </c>
+      <c r="E15" s="1">
+        <v>18441637.077</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>(B15-J14)/B14</f>
+        <v>1565.0301200000943</v>
+      </c>
+      <c r="C18">
+        <f>(C15-J14)/C14</f>
+        <v>906.79468000002203</v>
+      </c>
+      <c r="D18">
+        <f>(D15-J14)/D14</f>
+        <v>833.35514285715567</v>
+      </c>
+      <c r="E18">
+        <f>(E15-J14)/E14</f>
+        <v>847.37221600000555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,28 +724,28 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>8670386.5332999993</v>
+        <v>8671180.7280000001</v>
       </c>
       <c r="C4" s="1">
-        <v>8752399.9066700004</v>
+        <v>8753232.8049999997</v>
       </c>
       <c r="D4" s="1">
-        <v>8876659.7200000007</v>
+        <v>8876883.8159999996</v>
       </c>
       <c r="E4" s="1">
-        <v>9001015.1866699997</v>
+        <v>9001355.1669999994</v>
       </c>
       <c r="F4" s="1">
-        <v>9125726.5800000001</v>
+        <v>9125871.7799999993</v>
       </c>
       <c r="G4" s="1">
-        <v>9249752.4866700005</v>
+        <v>9248723.9509999994</v>
       </c>
       <c r="H4" s="1">
-        <v>9415005.6466700006</v>
+        <v>9413341.4010000005</v>
       </c>
       <c r="J4" s="1">
-        <v>8628270.3399999999</v>
+        <v>8630374.4010000005</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -562,35 +759,35 @@
       </c>
       <c r="B7">
         <f>(B4-J4)/B3</f>
-        <v>1684.6477319999785</v>
+        <v>1632.2530799999834</v>
       </c>
       <c r="C7">
         <f>(C4-J4)/C3</f>
-        <v>1655.0608889333407</v>
+        <v>1638.1120533333221</v>
       </c>
       <c r="D7">
         <f>(D4-J4)/D3</f>
-        <v>1655.9292000000055</v>
+        <v>1643.396099999994</v>
       </c>
       <c r="E7">
         <f>(E4-J4)/E3</f>
-        <v>1656.6437629777772</v>
+        <v>1648.8034044444396</v>
       </c>
       <c r="F7">
         <f>(F4-J4)/F3</f>
-        <v>1658.1874666666674</v>
+        <v>1651.657929999996</v>
       </c>
       <c r="G7">
         <f>(G4-J4)/G3</f>
-        <v>1657.285724453335</v>
+        <v>1648.9321333333303</v>
       </c>
       <c r="H7">
         <f>(H4-J4)/H3</f>
-        <v>1656.28485614737</v>
+        <v>1648.3515789473684</v>
       </c>
       <c r="J7">
         <f>SUM(B7:H7)/7</f>
-        <v>1660.5770901683536</v>
+        <v>1644.5008971512048</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -623,19 +820,19 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>8671186.0600000005</v>
+        <v>8671180.7280000001</v>
       </c>
       <c r="C15" s="1">
-        <v>8794613.3066700008</v>
+        <v>8794814.0940000005</v>
       </c>
       <c r="D15" s="1">
-        <v>8918932.9733300004</v>
+        <v>8918636.3579999991</v>
       </c>
       <c r="E15" s="1">
-        <v>9043501.5133299995</v>
+        <v>9043647.0850000009</v>
       </c>
       <c r="J15" s="1">
-        <v>8628906.7799999993</v>
+        <v>8630374.4010000005</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -649,23 +846,23 @@
       </c>
       <c r="B18">
         <f>(B15-J15)/B14</f>
-        <v>1691.1712000000477</v>
+        <v>1632.2530799999834</v>
       </c>
       <c r="C18">
         <f>(C15-J15)/C14</f>
-        <v>1657.0652667000145</v>
+        <v>1644.3969299999997</v>
       </c>
       <c r="D18">
         <f>(D15-J15)/D14</f>
-        <v>1657.2925333142919</v>
+        <v>1647.2111828571344</v>
       </c>
       <c r="E18">
         <f>(E15-J15)/E14</f>
-        <v>1658.3789333200007</v>
+        <v>1653.0907360000015</v>
       </c>
       <c r="J18">
         <f>SUM(B18:E18)/4</f>
-        <v>1665.9769833335886</v>
+        <v>1644.2379822142798</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -716,28 +913,28 @@
         <v>10</v>
       </c>
       <c r="B24" s="1">
-        <v>8670386.5332999993</v>
+        <v>8552767.3210000005</v>
       </c>
       <c r="C24" s="1">
-        <v>8752399.9066700004</v>
+        <v>8597682.3849999998</v>
       </c>
       <c r="D24" s="1">
-        <v>8876659.7200000007</v>
+        <v>8664171.4189999998</v>
       </c>
       <c r="E24" s="1">
-        <v>9001015.1866699997</v>
+        <v>8730814.9590000007</v>
       </c>
       <c r="F24" s="1">
-        <v>9125726.5800000001</v>
+        <v>8798512.4869999997</v>
       </c>
       <c r="G24" s="1">
-        <v>9249752.4866700005</v>
+        <v>8866177.1779999994</v>
       </c>
       <c r="H24" s="1">
-        <v>9415005.6466700006</v>
+        <v>8954777.9900000002</v>
       </c>
       <c r="J24" s="1">
-        <v>8628270.3399999999</v>
+        <v>8531229.0859999992</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -751,41 +948,49 @@
       </c>
       <c r="B27">
         <f>(B24-J24)/B23</f>
-        <v>1684.6477319999785</v>
+        <v>861.52940000005071</v>
       </c>
       <c r="C27">
         <f>(C24-J24)/C23</f>
-        <v>1655.0608889333407</v>
+        <v>886.04398666667441</v>
       </c>
       <c r="D27">
         <f>(D24-J24)/D23</f>
-        <v>1655.9292000000055</v>
+        <v>886.2822200000038</v>
       </c>
       <c r="E27">
         <f>(E24-J24)/E23</f>
-        <v>1656.6437629777772</v>
+        <v>887.04832444445128</v>
       </c>
       <c r="F27">
         <f>(F24-J24)/F23</f>
-        <v>1658.1874666666674</v>
+        <v>890.94467000000179</v>
       </c>
       <c r="G27">
         <f>(G24-J24)/G23</f>
-        <v>1657.285724453335</v>
+        <v>893.1949120000005</v>
       </c>
       <c r="H27">
         <f>(H24-J24)/H23</f>
-        <v>1656.28485614737</v>
+        <v>891.68190315789695</v>
       </c>
       <c r="J27">
         <f>SUM(B27:H27)/7</f>
-        <v>1660.5770901683536</v>
+        <v>885.24648803843991</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
+      <c r="J31">
+        <v>8506431.7390000001</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -812,19 +1017,19 @@
         <v>10</v>
       </c>
       <c r="B35" s="1">
-        <v>8671186.0600000005</v>
+        <v>8552767.3210000005</v>
       </c>
       <c r="C35" s="1">
-        <v>8794613.3066700008</v>
+        <v>8620017.8839999996</v>
       </c>
       <c r="D35" s="1">
-        <v>8918932.9733300004</v>
+        <v>8686818.7239999995</v>
       </c>
       <c r="E35" s="1">
-        <v>9043501.5133299995</v>
+        <v>8753424.5370000005</v>
       </c>
       <c r="J35" s="1">
-        <v>8628906.7799999993</v>
+        <v>8531229.0859999992</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -838,23 +1043,23 @@
       </c>
       <c r="B38">
         <f>(B35-J35)/B34</f>
-        <v>1691.1712000000477</v>
+        <v>861.52940000005071</v>
       </c>
       <c r="C38">
         <f>(C35-J35)/C34</f>
-        <v>1657.0652667000145</v>
+        <v>887.88798000000418</v>
       </c>
       <c r="D38">
         <f>(D35-J35)/D34</f>
-        <v>1657.2925333142919</v>
+        <v>889.08364571428729</v>
       </c>
       <c r="E38">
         <f>(E35-J35)/E34</f>
-        <v>1658.3789333200007</v>
+        <v>888.78180400000508</v>
       </c>
       <c r="J38">
         <f>SUM(B38:E38)/4</f>
-        <v>1665.9769833335886</v>
+        <v>881.82070742858684</v>
       </c>
     </row>
   </sheetData>
@@ -863,12 +1068,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,6 +1086,7 @@
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -924,28 +1130,28 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>18337256.491</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>18375869.535999998</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>18427300.673</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>18472670.052000001</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>18493557.265999999</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>18556089.388999999</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>18592454.977000002</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>18308798.851</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -954,31 +1160,31 @@
       </c>
       <c r="B7">
         <f>(B4-J4)/B3</f>
-        <v>0</v>
+        <v>1138.3056000000238</v>
       </c>
       <c r="C7">
         <f>(C4-J4)/C3</f>
-        <v>0</v>
+        <v>894.27579999998215</v>
       </c>
       <c r="D7">
         <f>(D4-J4)/D3</f>
-        <v>0</v>
+        <v>790.01214666667079</v>
       </c>
       <c r="E7">
         <f>(E4-J4)/E3</f>
-        <v>0</v>
+        <v>728.31644888889457</v>
       </c>
       <c r="F7">
         <f>(F4-J4)/F3</f>
-        <v>0</v>
+        <v>615.86138333333031</v>
       </c>
       <c r="G7">
         <f>(G4-J4)/G3</f>
-        <v>0</v>
+        <v>659.44143466666344</v>
       </c>
       <c r="H7">
         <f>(H4-J4)/H3</f>
-        <v>0</v>
+        <v>597.17079157895159</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1008,7 +1214,7 @@
         <v>250</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>18308798.851</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1016,16 +1222,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>18337256.491</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>18391399.622000001</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>18445358.588</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>18487790.798</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,19 +1240,19 @@
       </c>
       <c r="B18">
         <f>(B15-J14)/B14</f>
-        <v>0</v>
+        <v>1138.3056000000238</v>
       </c>
       <c r="C18">
         <f>(C15-J14)/C14</f>
-        <v>0</v>
+        <v>826.00771000001578</v>
       </c>
       <c r="D18">
         <f>(D15-J14)/D14</f>
-        <v>0</v>
+        <v>780.34135428571278</v>
       </c>
       <c r="E18">
         <f>(E15-J14)/E14</f>
-        <v>0</v>
+        <v>715.96778800000254</v>
       </c>
     </row>
   </sheetData>
@@ -1054,8 +1260,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>